<commit_message>
age comparison and age frequency plots. Hope the deleted files get ignored.
</commit_message>
<xml_diff>
--- a/AECL520/NewFams.xlsx
+++ b/AECL520/NewFams.xlsx
@@ -514,10 +514,10 @@
         <v>1228.6700000000001</v>
       </c>
       <c>
-        <v>220.25399999999999</v>
-      </c>
-      <c>
-        <v>734515.32799999998</v>
+        <v>222.82300000000001</v>
+      </c>
+      <c>
+        <v>194.042</v>
       </c>
     </row>
     <row>
@@ -531,10 +531,10 @@
         <v>773.88</v>
       </c>
       <c>
-        <v>249.166</v>
-      </c>
-      <c>
-        <v>631832.89399999997</v>
+        <v>250.298</v>
+      </c>
+      <c>
+        <v>175.42099999999999</v>
       </c>
     </row>
     <row>
@@ -548,10 +548,10 @@
         <v>389.36000000000001</v>
       </c>
       <c>
-        <v>278.11700000000002</v>
-      </c>
-      <c>
-        <v>419673.96899999998</v>
+        <v>278.43599999999998</v>
+      </c>
+      <c>
+        <v>122.901</v>
       </c>
     </row>
     <row>
@@ -565,10 +565,10 @@
         <v>2119.46</v>
       </c>
       <c>
-        <v>212.75899999999999</v>
-      </c>
-      <c>
-        <v>1160910.953</v>
+        <v>215.22999999999999</v>
+      </c>
+      <c>
+        <v>300.529</v>
       </c>
     </row>
     <row>
@@ -582,10 +582,10 @@
         <v>1372.1199999999999</v>
       </c>
       <c>
-        <v>244.916</v>
-      </c>
-      <c>
-        <v>1072599.2109999999</v>
+        <v>246.00999999999999</v>
+      </c>
+      <c>
+        <v>294.76100000000002</v>
       </c>
     </row>
     <row>
@@ -599,10 +599,10 @@
         <v>724.88</v>
       </c>
       <c>
-        <v>276.54700000000003</v>
-      </c>
-      <c>
-        <v>770223.53599999996</v>
+        <v>276.86000000000001</v>
+      </c>
+      <c>
+        <v>224.809</v>
       </c>
     </row>
     <row>
@@ -616,10 +616,10 @@
         <v>2768.6399999999999</v>
       </c>
       <c>
-        <v>205.202</v>
-      </c>
-      <c>
-        <v>1384048.4750000001</v>
+        <v>207.488</v>
+      </c>
+      <c>
+        <v>350.33499999999998</v>
       </c>
     </row>
     <row>
@@ -633,10 +633,10 @@
         <v>1831.0999999999999</v>
       </c>
       <c>
-        <v>240.47</v>
-      </c>
-      <c>
-        <v>1366633.3859999999</v>
+        <v>241.49700000000001</v>
+      </c>
+      <c>
+        <v>371.363</v>
       </c>
     </row>
     <row>
@@ -650,10 +650,10 @@
         <v>1010.68</v>
       </c>
       <c>
-        <v>274.82999999999998</v>
-      </c>
-      <c>
-        <v>1057138.0660000001</v>
+        <v>275.13400000000001</v>
+      </c>
+      <c>
+        <v>307.411</v>
       </c>
     </row>
     <row>
@@ -667,10 +667,10 @@
         <v>3248.98</v>
       </c>
       <c>
-        <v>197.78800000000001</v>
-      </c>
-      <c>
-        <v>1479943.067</v>
+        <v>199.81100000000001</v>
+      </c>
+      <c>
+        <v>365.654</v>
       </c>
     </row>
     <row>
@@ -684,10 +684,10 @@
         <v>2182.2800000000002</v>
       </c>
       <c>
-        <v>235.89400000000001</v>
-      </c>
-      <c>
-        <v>1551541.1000000001</v>
+        <v>236.82400000000001</v>
+      </c>
+      <c>
+        <v>416.51100000000002</v>
       </c>
     </row>
     <row>
@@ -701,10 +701,10 @@
         <v>1251.0799999999999</v>
       </c>
       <c>
-        <v>272.95100000000002</v>
-      </c>
-      <c>
-        <v>1286096.273</v>
+        <v>273.24000000000001</v>
+      </c>
+      <c>
+        <v>372.44900000000001</v>
       </c>
     </row>
     <row>
@@ -718,10 +718,10 @@
         <v>3614.1399999999999</v>
       </c>
       <c>
-        <v>190.703</v>
-      </c>
-      <c>
-        <v>1501311.743</v>
+        <v>192.405</v>
+      </c>
+      <c>
+        <v>361.70400000000001</v>
       </c>
     </row>
     <row>
@@ -735,10 +735,10 @@
         <v>2452.4200000000001</v>
       </c>
       <c>
-        <v>231.268</v>
-      </c>
-      <c>
-        <v>1658491.0220000001</v>
+        <v>232.07499999999999</v>
+      </c>
+      <c>
+        <v>439.51100000000002</v>
       </c>
     </row>
     <row>
@@ -752,10 +752,10 @@
         <v>1450.6700000000001</v>
       </c>
       <c>
-        <v>270.89299999999997</v>
-      </c>
-      <c>
-        <v>1463004.3670000001</v>
+        <v>271.161</v>
+      </c>
+      <c>
+        <v>421.73099999999999</v>
       </c>
     </row>
     <row>
@@ -769,10 +769,10 @@
         <v>3902.8200000000002</v>
       </c>
       <c>
-        <v>184.07499999999999</v>
-      </c>
-      <c>
-        <v>1482586.2509999999</v>
+        <v>185.43000000000001</v>
+      </c>
+      <c>
+        <v>348.24200000000002</v>
       </c>
     </row>
     <row>
@@ -786,10 +786,10 @@
         <v>2664.0300000000002</v>
       </c>
       <c>
-        <v>226.673</v>
-      </c>
-      <c>
-        <v>1712520.48</v>
+        <v>227.33699999999999</v>
+      </c>
+      <c>
+        <v>447.78699999999998</v>
       </c>
     </row>
     <row>
@@ -803,10 +803,10 @@
         <v>1614.4000000000001</v>
       </c>
       <c>
-        <v>268.63400000000001</v>
-      </c>
-      <c>
-        <v>1594052.0430000001</v>
+        <v>268.87400000000002</v>
+      </c>
+      <c>
+        <v>457.13999999999999</v>
       </c>
     </row>
     <row>
@@ -820,10 +820,10 @@
         <v>4142.6999999999998</v>
       </c>
       <c>
-        <v>177.929</v>
-      </c>
-      <c>
-        <v>1444308.4339999999</v>
+        <v>178.94200000000001</v>
+      </c>
+      <c>
+        <v>330.91500000000002</v>
       </c>
     </row>
     <row>
@@ -837,10 +837,10 @@
         <v>2835.8899999999999</v>
       </c>
       <c>
-        <v>222.16900000000001</v>
-      </c>
-      <c>
-        <v>1732839.25</v>
+        <v>222.679</v>
+      </c>
+      <c>
+        <v>446.96600000000001</v>
       </c>
     </row>
     <row>
@@ -854,10 +854,10 @@
         <v>1747.9300000000001</v>
       </c>
       <c>
-        <v>266.14699999999999</v>
-      </c>
-      <c>
-        <v>1685803.0900000001</v>
+        <v>266.35000000000002</v>
+      </c>
+      <c>
+        <v>480.65199999999999</v>
       </c>
     </row>
     <row>
@@ -871,10 +871,10 @@
         <v>4355.0799999999999</v>
       </c>
       <c>
-        <v>172.14400000000001</v>
-      </c>
-      <c>
-        <v>1396667.517</v>
+        <v>172.84100000000001</v>
+      </c>
+      <c>
+        <v>312.322</v>
       </c>
     </row>
     <row>
@@ -888,10 +888,10 @@
         <v>2984.3800000000001</v>
       </c>
       <c>
-        <v>217.738</v>
-      </c>
-      <c>
-        <v>1733055.6059999999</v>
+        <v>218.09399999999999</v>
+      </c>
+      <c>
+        <v>440.91699999999997</v>
       </c>
     </row>
     <row>
@@ -905,10 +905,10 @@
         <v>1858.21</v>
       </c>
       <c>
-        <v>263.375</v>
-      </c>
-      <c>
-        <v>1745368.9439999999</v>
+        <v>263.53199999999998</v>
+      </c>
+      <c>
+        <v>494.36099999999999</v>
       </c>
     </row>
     <row>
@@ -922,10 +922,10 @@
         <v>4563.4899999999998</v>
       </c>
       <c>
-        <v>166.28800000000001</v>
-      </c>
-      <c>
-        <v>1340958.6340000001</v>
+        <v>166.69999999999999</v>
+      </c>
+      <c>
+        <v>292.46300000000002</v>
       </c>
     </row>
     <row>
@@ -939,10 +939,10 @@
         <v>3127.8699999999999</v>
       </c>
       <c>
-        <v>213.131</v>
-      </c>
-      <c>
-        <v>1720843.852</v>
+        <v>213.34100000000001</v>
+      </c>
+      <c>
+        <v>431.53399999999999</v>
       </c>
     </row>
     <row>
@@ -956,10 +956,10 @@
         <v>1956.28</v>
       </c>
       <c>
-        <v>260.13400000000001</v>
-      </c>
-      <c>
-        <v>1780880.449</v>
+        <v>260.23399999999998</v>
+      </c>
+      <c>
+        <v>500.47800000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>